<commit_message>
Problema de desempenho - controlado
</commit_message>
<xml_diff>
--- a/RelatorioContasCorrente.xlsx
+++ b/RelatorioContasCorrente.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1108" uniqueCount="11">
   <si>
     <t>Account ID</t>
   </si>
@@ -131,6 +131,21 @@
   </si>
   <si>
     <t>Timestamp</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Pagamento</t>
+  </si>
+  <si>
+    <t>Driver 12</t>
+  </si>
+  <si>
+    <t>Recebimento</t>
+  </si>
+  <si>
+    <t>Driver 60</t>
   </si>
 </sst>
 </file>
@@ -175,7 +190,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -201,6 +216,1246 @@
         <v>5</v>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F2" t="n">
+        <v>45219.81036674768</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F3" t="n">
+        <v>45219.8103728125</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>45219.81037900463</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>45219.810385046294</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45219.81039144676</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F7" t="n">
+        <v>45219.81039744213</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F8" t="n">
+        <v>45219.81040354167</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F9" t="n">
+        <v>45219.81040967593</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>45219.81041575231</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F11" t="n">
+        <v>45219.81042224537</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>45219.81042821759</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F13" t="n">
+        <v>45219.810434259256</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F14" t="n">
+        <v>45219.81044023148</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F15" t="n">
+        <v>45219.81044642361</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F16" t="n">
+        <v>45219.81045255787</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F17" t="n">
+        <v>45219.81045872685</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F18" t="n">
+        <v>45219.810465092596</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F19" t="n">
+        <v>45219.8104712037</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F20" t="n">
+        <v>45219.8104771875</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F21" t="n">
+        <v>45219.810483402776</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F22" t="n">
+        <v>45219.81048956019</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F23" t="n">
+        <v>45219.81049563657</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F24" t="n">
+        <v>45219.810501631946</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F25" t="n">
+        <v>45219.81050759259</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F26" t="n">
+        <v>45219.81051355324</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F27" t="n">
+        <v>45219.81057768519</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F28" t="n">
+        <v>45219.81058358796</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F29" t="n">
+        <v>45219.81058950232</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F30" t="n">
+        <v>45219.81059533565</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F31" t="n">
+        <v>45219.810601157405</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F32" t="n">
+        <v>45219.8106071875</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F33" t="n">
+        <v>45219.81061314815</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>6</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F34" t="n">
+        <v>45219.81061920139</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F35" t="n">
+        <v>45219.810625335645</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F36" t="n">
+        <v>45219.81063119213</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F37" t="n">
+        <v>45219.81063714121</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F38" t="n">
+        <v>45219.810643136574</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F39" t="n">
+        <v>45219.81064920139</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>7</v>
+      </c>
+      <c r="D40" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F40" t="n">
+        <v>45219.81065508102</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F41" t="n">
+        <v>45219.81066106482</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>6</v>
+      </c>
+      <c r="B42" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" t="s">
+        <v>7</v>
+      </c>
+      <c r="D42" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F42" t="n">
+        <v>45219.81066708334</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F43" t="n">
+        <v>45219.81067292824</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" t="s">
+        <v>6</v>
+      </c>
+      <c r="C44" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F44" t="n">
+        <v>45219.81067912037</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>6</v>
+      </c>
+      <c r="B45" t="s">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>7</v>
+      </c>
+      <c r="D45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F45" t="n">
+        <v>45219.810685069446</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>6</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F46" t="n">
+        <v>45219.81069097222</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F47" t="n">
+        <v>45219.810696886576</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F48" t="n">
+        <v>45219.81070278935</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>6</v>
+      </c>
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="s">
+        <v>7</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F49" t="n">
+        <v>45219.81070884259</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>6</v>
+      </c>
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F50" t="n">
+        <v>45219.81071478009</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>6</v>
+      </c>
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" t="s">
+        <v>7</v>
+      </c>
+      <c r="D51" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F51" t="n">
+        <v>45219.81072072917</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>6</v>
+      </c>
+      <c r="B52" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F52" t="n">
+        <v>45219.81072673611</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53" t="s">
+        <v>7</v>
+      </c>
+      <c r="D53" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F53" t="n">
+        <v>45219.810732708334</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>6</v>
+      </c>
+      <c r="B54" t="s">
+        <v>6</v>
+      </c>
+      <c r="C54" t="s">
+        <v>7</v>
+      </c>
+      <c r="D54" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F54" t="n">
+        <v>45219.81073871528</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>6</v>
+      </c>
+      <c r="C55" t="s">
+        <v>7</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F55" t="n">
+        <v>45219.8107447338</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>6</v>
+      </c>
+      <c r="C56" t="s">
+        <v>7</v>
+      </c>
+      <c r="D56" t="s">
+        <v>10</v>
+      </c>
+      <c r="E56" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F56" t="n">
+        <v>45219.81075064815</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" t="s">
+        <v>6</v>
+      </c>
+      <c r="C57" t="s">
+        <v>7</v>
+      </c>
+      <c r="D57" t="s">
+        <v>10</v>
+      </c>
+      <c r="E57" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F57" t="n">
+        <v>45219.81075660879</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>6</v>
+      </c>
+      <c r="B58" t="s">
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>7</v>
+      </c>
+      <c r="D58" t="s">
+        <v>10</v>
+      </c>
+      <c r="E58" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F58" t="n">
+        <v>45219.810762546294</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>6</v>
+      </c>
+      <c r="B59" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" t="s">
+        <v>10</v>
+      </c>
+      <c r="E59" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F59" t="n">
+        <v>45219.810768564814</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>6</v>
+      </c>
+      <c r="B60" t="s">
+        <v>6</v>
+      </c>
+      <c r="C60" t="s">
+        <v>7</v>
+      </c>
+      <c r="D60" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F60" t="n">
+        <v>45219.810774791666</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>6</v>
+      </c>
+      <c r="B61" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" t="s">
+        <v>7</v>
+      </c>
+      <c r="D61" t="s">
+        <v>10</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F61" t="n">
+        <v>45219.81078076389</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>6</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" t="s">
+        <v>7</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F62" t="n">
+        <v>45219.81078664352</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>6</v>
+      </c>
+      <c r="B63" t="s">
+        <v>6</v>
+      </c>
+      <c r="C63" t="s">
+        <v>7</v>
+      </c>
+      <c r="D63" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F63" t="n">
+        <v>45219.81079267361</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -439,30 +1694,530 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F2" t="n">
+        <v>45219.81036674768</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F3" t="n">
+        <v>45219.8103728125</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>45219.81037900463</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>45219.810385046294</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45219.81039144676</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F7" t="n">
+        <v>45219.81039744213</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F8" t="n">
+        <v>45219.81040354167</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F9" t="n">
+        <v>45219.81040967593</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>45219.81041575231</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F11" t="n">
+        <v>45219.81042224537</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>45219.81042821759</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F13" t="n">
+        <v>45219.810434259256</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F14" t="n">
+        <v>45219.81044023148</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F15" t="n">
+        <v>45219.81044642361</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F16" t="n">
+        <v>45219.81045255787</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F17" t="n">
+        <v>45219.81045872685</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F18" t="n">
+        <v>45219.810465092596</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F19" t="n">
+        <v>45219.8104712037</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F20" t="n">
+        <v>45219.8104771875</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F21" t="n">
+        <v>45219.810483402776</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F22" t="n">
+        <v>45219.81048956019</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F23" t="n">
+        <v>45219.81049563657</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F24" t="n">
+        <v>45219.810501631946</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F25" t="n">
+        <v>45219.81050759259</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F26" t="n">
+        <v>45219.81051355324</v>
       </c>
     </row>
   </sheetData>
@@ -2188,30 +3943,770 @@
 
 <file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+  <dimension ref="A1:F38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F2" t="n">
+        <v>45219.81057768519</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F3" t="n">
+        <v>45219.81058358796</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>45219.81058950232</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>45219.81059533565</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F6" t="n">
+        <v>45219.810601157405</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F7" t="n">
+        <v>45219.8106071875</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F8" t="n">
+        <v>45219.81061314815</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F9" t="n">
+        <v>45219.81061920139</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>45219.810625335645</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F11" t="n">
+        <v>45219.81063119213</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F12" t="n">
+        <v>45219.81063714121</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F13" t="n">
+        <v>45219.810643136574</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F14" t="n">
+        <v>45219.81064920139</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F15" t="n">
+        <v>45219.81065508102</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F16" t="n">
+        <v>45219.81066106482</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F17" t="n">
+        <v>45219.81066708334</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F18" t="n">
+        <v>45219.81067292824</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F19" t="n">
+        <v>45219.81067912037</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F20" t="n">
+        <v>45219.810685069446</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" t="s">
+        <v>6</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F21" t="n">
+        <v>45219.81069097222</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F22" t="n">
+        <v>45219.810696886576</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>6</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F23" t="n">
+        <v>45219.81070278935</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F24" t="n">
+        <v>45219.81070884259</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F25" t="n">
+        <v>45219.81071478009</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F26" t="n">
+        <v>45219.81072072917</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F27" t="n">
+        <v>45219.81072673611</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>6</v>
+      </c>
+      <c r="C28" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F28" t="n">
+        <v>45219.810732708334</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F29" t="n">
+        <v>45219.81073871528</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F30" t="n">
+        <v>45219.8107447338</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F31" t="n">
+        <v>45219.81075064815</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F32" t="n">
+        <v>45219.81075660879</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F33" t="n">
+        <v>45219.810762546294</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" t="s">
+        <v>10</v>
+      </c>
+      <c r="E34" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F34" t="n">
+        <v>45219.810768564814</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F35" t="n">
+        <v>45219.810774791666</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F36" t="n">
+        <v>45219.81078076389</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F37" t="n">
+        <v>45219.81078664352</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="F38" t="n">
+        <v>45219.81079267361</v>
       </c>
     </row>
   </sheetData>

</xml_diff>